<commit_message>
maj EP09 et EP10 part 1
</commit_message>
<xml_diff>
--- a/conf/EP10.xlsx
+++ b/conf/EP10.xlsx
@@ -1885,6 +1885,1071 @@
       </c>
       <c r="O30" s="3" t="inlineStr"/>
     </row>
+    <row r="31" customHeight="1" ht="20">
+      <c r="A31" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">RC034               </t>
+          </r>
+        </is>
+      </c>
+      <c r="B31" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Expositions sur les organismes publics hors </t>
+          </r>
+        </is>
+      </c>
+      <c r="C31" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="D31" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="E31" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="F31" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="G31" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="H31" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="I31" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="J31" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="K31" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="L31" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="M31" s="9" t="inlineStr"/>
+      <c r="N31" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="O31" s="3" t="inlineStr"/>
+    </row>
+    <row r="32" customHeight="1" ht="20">
+      <c r="A32" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">RC035               </t>
+          </r>
+        </is>
+      </c>
+      <c r="B32" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Expositions sur les Banques Multilatérales de </t>
+          </r>
+        </is>
+      </c>
+      <c r="C32" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="D32" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="E32" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="F32" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="G32" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="H32" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="I32" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="J32" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="K32" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="L32" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="M32" s="9" t="inlineStr"/>
+      <c r="N32" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="O32" s="3" t="inlineStr"/>
+    </row>
+    <row r="33" customHeight="1" ht="20">
+      <c r="A33" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">RC036               </t>
+          </r>
+        </is>
+      </c>
+      <c r="B33" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Expositions sur les institutions financières	                                                                                                                                                           </t>
+          </r>
+        </is>
+      </c>
+      <c r="C33" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="D33" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="E33" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="F33" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="G33" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="H33" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="I33" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="J33" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="K33" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="L33" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="M33" s="9" t="inlineStr"/>
+      <c r="N33" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="O33" s="3" t="inlineStr"/>
+    </row>
+    <row r="34" customHeight="1" ht="20">
+      <c r="A34" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">RC037               </t>
+          </r>
+        </is>
+      </c>
+      <c r="B34" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Expositions sur les entreprises; dont :	                                                                                                                                                                </t>
+          </r>
+        </is>
+      </c>
+      <c r="C34" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="D34" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="E34" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="F34" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="G34" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="H34" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="I34" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="J34" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="K34" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="L34" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="M34" s="9" t="inlineStr"/>
+      <c r="N34" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="O34" s="3" t="inlineStr"/>
+    </row>
+    <row r="35" customHeight="1" ht="20">
+      <c r="A35" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">RC038               </t>
+          </r>
+        </is>
+      </c>
+      <c r="B35" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">     - PME assimilables à des entreprises	                                                                                                                                                              </t>
+          </r>
+        </is>
+      </c>
+      <c r="C35" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="D35" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="E35" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="F35" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="G35" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="H35" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="I35" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="J35" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="K35" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="L35" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="M35" s="9" t="inlineStr"/>
+      <c r="N35" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="O35" s="3" t="inlineStr"/>
+    </row>
+    <row r="36" customHeight="1" ht="20">
+      <c r="A36" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">RC039               </t>
+          </r>
+        </is>
+      </c>
+      <c r="B36" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">     - Autres entreprises	                                                                                                                                                                              </t>
+          </r>
+        </is>
+      </c>
+      <c r="C36" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="D36" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="E36" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="F36" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="G36" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="H36" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="I36" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="J36" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="K36" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="L36" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="M36" s="9" t="inlineStr"/>
+      <c r="N36" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="O36" s="3" t="inlineStr"/>
+    </row>
+    <row r="37" customHeight="1" ht="20">
+      <c r="A37" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">RC040               </t>
+          </r>
+        </is>
+      </c>
+      <c r="B37" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Expositions sur la clientèle de détail	                                                                                                                                                                 </t>
+          </r>
+        </is>
+      </c>
+      <c r="C37" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="D37" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="E37" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="F37" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="G37" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="H37" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="I37" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="J37" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="K37" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="L37" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="M37" s="9" t="inlineStr"/>
+      <c r="N37" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="O37" s="3" t="inlineStr"/>
+    </row>
+    <row r="38" customHeight="1" ht="20">
+      <c r="A38" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">RC041               </t>
+          </r>
+        </is>
+      </c>
+      <c r="B38" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">     - PME assimilables à la clientèle de détail	                                                                                                                                                       </t>
+          </r>
+        </is>
+      </c>
+      <c r="C38" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="D38" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="E38" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="F38" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="G38" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="H38" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="I38" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="J38" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="K38" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="L38" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="M38" s="9" t="inlineStr"/>
+      <c r="N38" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="O38" s="3" t="inlineStr"/>
+    </row>
+    <row r="39" customHeight="1" ht="20">
+      <c r="A39" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">RC042               </t>
+          </r>
+        </is>
+      </c>
+      <c r="B39" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">     - Autres clientèle de détail	                                                                                                                                                                      </t>
+          </r>
+        </is>
+      </c>
+      <c r="C39" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="D39" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="E39" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="F39" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="G39" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="H39" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="I39" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="J39" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="K39" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="L39" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="M39" s="9" t="inlineStr"/>
+      <c r="N39" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="O39" s="3" t="inlineStr"/>
+    </row>
+    <row r="40" customHeight="1" ht="20">
+      <c r="A40" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">RC043               </t>
+          </r>
+        </is>
+      </c>
+      <c r="B40" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Expositions sur les prêts garantis par l'immobilier </t>
+          </r>
+        </is>
+      </c>
+      <c r="C40" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="D40" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="E40" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="F40" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="G40" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="H40" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="I40" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="J40" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="K40" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="L40" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="M40" s="9" t="inlineStr"/>
+      <c r="N40" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="O40" s="3" t="inlineStr"/>
+    </row>
+    <row r="41" customHeight="1" ht="20">
+      <c r="A41" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">RC044               </t>
+          </r>
+        </is>
+      </c>
+      <c r="B41" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Expositions sur les prêts garantis par l'immobilier </t>
+          </r>
+        </is>
+      </c>
+      <c r="C41" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="D41" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="E41" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="F41" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="G41" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="H41" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="I41" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="J41" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="K41" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="L41" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="M41" s="9" t="inlineStr"/>
+      <c r="N41" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="O41" s="3" t="inlineStr"/>
+    </row>
+    <row r="42" customHeight="1" ht="20">
+      <c r="A42" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">RC045               </t>
+          </r>
+        </is>
+      </c>
+      <c r="B42" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">     - PME	                                                                                                                                                                                             </t>
+          </r>
+        </is>
+      </c>
+      <c r="C42" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="D42" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="E42" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="F42" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="G42" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="H42" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="I42" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="J42" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="K42" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="L42" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="M42" s="9" t="inlineStr"/>
+      <c r="N42" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="O42" s="3" t="inlineStr"/>
+    </row>
+    <row r="43" customHeight="1" ht="20">
+      <c r="A43" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">RC046               </t>
+          </r>
+        </is>
+      </c>
+      <c r="B43" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">     - Autres expositions sur les prêts garantis par </t>
+          </r>
+        </is>
+      </c>
+      <c r="C43" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="D43" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="E43" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="F43" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="G43" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="H43" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="I43" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="J43" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="K43" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="L43" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="M43" s="9" t="inlineStr"/>
+      <c r="N43" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="O43" s="3" t="inlineStr"/>
+    </row>
+    <row r="44" customHeight="1" ht="20">
+      <c r="A44" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">RC047               </t>
+          </r>
+        </is>
+      </c>
+      <c r="B44" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">Autres actifs	                                                                                                                                                                                          </t>
+          </r>
+        </is>
+      </c>
+      <c r="C44" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="D44" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="E44" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="F44" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="G44" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="H44" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="I44" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="J44" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="K44" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="L44" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="M44" s="9" t="inlineStr"/>
+      <c r="N44" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="O44" s="3" t="inlineStr"/>
+    </row>
+    <row r="45" customHeight="1" ht="20">
+      <c r="A45" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">RC048               </t>
+          </r>
+        </is>
+      </c>
+      <c r="B45" s="7" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">TOTAL EXPOSITIONS SUR LES AUTRES </t>
+          </r>
+        </is>
+      </c>
+      <c r="C45" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="D45" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0.0</t>
+          </r>
+        </is>
+      </c>
+      <c r="E45" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="F45" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="G45" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="H45" s="8" t="inlineStr">
+        <is>
+          <r>
+            <t xml:space="preserve">0</t>
+          </r>
+        </is>
+      </c>
+      <c r="I45" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="J45" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="K45" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="L45" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="M45" s="9" t="inlineStr"/>
+      <c r="N45" s="8" t="inlineStr">
+        <is/>
+      </c>
+      <c r="O45" s="3" t="inlineStr"/>
+    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:L1"/>
@@ -1923,6 +2988,21 @@
     <mergeCell ref="A28:N28"/>
     <mergeCell ref="B29:N29"/>
     <mergeCell ref="L30:M30"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="L45:M45"/>
   </mergeCells>
   <pageMargins left="0.0" right="0.0" top="0.0" bottom="0.0" header="0.0" footer="0.0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>